<commit_message>
Delete Functional Requirements from SRS TeamPassionFruit.docx, Edit in 8. Logged user tries to create post from ScenariosPassionFruit.xlsx
</commit_message>
<xml_diff>
--- a/Docs/ScenariosPassionFruit.xlsx
+++ b/Docs/ScenariosPassionFruit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\SoftuniQA_Automation\GitHub TeamWork\Teamwork\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerganka\Desktop\TeamWork_ForkRepo\Teamwork\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,10 +197,10 @@
     <t xml:space="preserve">1. Start Browser     2. Navigate to  URL  http://localhost:60634/Article/List    3. Chech the user is logged     4. Click on Article Heading            5.  View Article Details Page  6.Click on Edit button    </t>
   </si>
   <si>
-    <t>Redirect to Create Article page. Registered user can create posts</t>
+    <t>1. Start Browser     2. Navigate to  URL  http://localhost:60634/Article/List    3. Check the user is logged     4. Click on Create button     5. Navigate to URL       http://localhost:60634/Article/List     6. Check the author name of last post</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Start Browser     2. Navigate to  URL  http://localhost:60634/Article/List    3. Check the user is logged     4. Click on Create button      </t>
+    <t>Redirect to Create Article page. Registered user can create posts. The name of last post's author must be the name of the user</t>
   </si>
 </sst>
 </file>
@@ -849,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I942"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,10 +1050,10 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I9" s="10"/>
     </row>

</xml_diff>